<commit_message>
added technicals and its flags to NEWPROD_env_sample file
</commit_message>
<xml_diff>
--- a/technical_logs.xlsx
+++ b/technical_logs.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -1726,6 +1726,4386 @@
         <v>93.18000000000001</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:44:46</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="D44" t="n">
+        <v>84.7</v>
+      </c>
+      <c r="E44" t="n">
+        <v>82.20999999999999</v>
+      </c>
+      <c r="F44" t="n">
+        <v>57.92</v>
+      </c>
+      <c r="G44" t="n">
+        <v>9.720000000000001</v>
+      </c>
+      <c r="H44" t="n">
+        <v>81.73999999999999</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:45:11</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>86.90000000000001</v>
+      </c>
+      <c r="D45" t="n">
+        <v>84.89</v>
+      </c>
+      <c r="E45" t="n">
+        <v>82.34999999999999</v>
+      </c>
+      <c r="F45" t="n">
+        <v>56.78</v>
+      </c>
+      <c r="G45" t="n">
+        <v>9.69</v>
+      </c>
+      <c r="H45" t="n">
+        <v>81.75</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:45:36</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>86.95</v>
+      </c>
+      <c r="D46" t="n">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="E46" t="n">
+        <v>82.34999999999999</v>
+      </c>
+      <c r="F46" t="n">
+        <v>56.86</v>
+      </c>
+      <c r="G46" t="n">
+        <v>9.69</v>
+      </c>
+      <c r="H46" t="n">
+        <v>81.76000000000001</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:46:32</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>93.05</v>
+      </c>
+      <c r="D47" t="n">
+        <v>86.79000000000001</v>
+      </c>
+      <c r="E47" t="n">
+        <v>83.13</v>
+      </c>
+      <c r="F47" t="n">
+        <v>64.66</v>
+      </c>
+      <c r="G47" t="n">
+        <v>11.57</v>
+      </c>
+      <c r="H47" t="n">
+        <v>81.88</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:46:56</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="D48" t="n">
+        <v>88.16</v>
+      </c>
+      <c r="E48" t="n">
+        <v>83.48</v>
+      </c>
+      <c r="F48" t="n">
+        <v>70.72</v>
+      </c>
+      <c r="G48" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="H48" t="n">
+        <v>82.12</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:48:21</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>90.25</v>
+      </c>
+      <c r="D49" t="n">
+        <v>89.23999999999999</v>
+      </c>
+      <c r="E49" t="n">
+        <v>85</v>
+      </c>
+      <c r="F49" t="n">
+        <v>55.84</v>
+      </c>
+      <c r="G49" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="H49" t="n">
+        <v>82.31999999999999</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:49:46</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550CE</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>95</v>
+      </c>
+      <c r="D50" t="n">
+        <v>92.62</v>
+      </c>
+      <c r="E50" t="n">
+        <v>96.44</v>
+      </c>
+      <c r="F50" t="n">
+        <v>47.67</v>
+      </c>
+      <c r="G50" t="n">
+        <v>19.71</v>
+      </c>
+      <c r="H50" t="n">
+        <v>105.7</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:50:12</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550CE</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>100.35</v>
+      </c>
+      <c r="D51" t="n">
+        <v>94.28</v>
+      </c>
+      <c r="E51" t="n">
+        <v>96.09</v>
+      </c>
+      <c r="F51" t="n">
+        <v>52.38</v>
+      </c>
+      <c r="G51" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="H51" t="n">
+        <v>105.67</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:50:37</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550CE</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>99.2</v>
+      </c>
+      <c r="D52" t="n">
+        <v>94.05</v>
+      </c>
+      <c r="E52" t="n">
+        <v>96.03</v>
+      </c>
+      <c r="F52" t="n">
+        <v>51.42</v>
+      </c>
+      <c r="G52" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="H52" t="n">
+        <v>105.64</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:51:32</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>NIFTY2611325650PE</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>110.05</v>
+      </c>
+      <c r="D53" t="n">
+        <v>113.3</v>
+      </c>
+      <c r="E53" t="n">
+        <v>113.44</v>
+      </c>
+      <c r="F53" t="n">
+        <v>47.78</v>
+      </c>
+      <c r="G53" t="n">
+        <v>11.48</v>
+      </c>
+      <c r="H53" t="n">
+        <v>104.93</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:52:26</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>NIFTY2611325650PE</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>115.65</v>
+      </c>
+      <c r="D54" t="n">
+        <v>113.76</v>
+      </c>
+      <c r="E54" t="n">
+        <v>113.73</v>
+      </c>
+      <c r="F54" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="G54" t="n">
+        <v>10.68</v>
+      </c>
+      <c r="H54" t="n">
+        <v>104.97</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:53:50</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>86.90000000000001</v>
+      </c>
+      <c r="D55" t="n">
+        <v>85.45</v>
+      </c>
+      <c r="E55" t="n">
+        <v>85.48999999999999</v>
+      </c>
+      <c r="F55" t="n">
+        <v>52.54</v>
+      </c>
+      <c r="G55" t="n">
+        <v>11.34</v>
+      </c>
+      <c r="H55" t="n">
+        <v>82.33</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:54:16</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>88.05</v>
+      </c>
+      <c r="D56" t="n">
+        <v>85.84</v>
+      </c>
+      <c r="E56" t="n">
+        <v>85.66</v>
+      </c>
+      <c r="F56" t="n">
+        <v>53.64</v>
+      </c>
+      <c r="G56" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="H56" t="n">
+        <v>82.34</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:54:41</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>90.40000000000001</v>
+      </c>
+      <c r="D57" t="n">
+        <v>86.31</v>
+      </c>
+      <c r="E57" t="n">
+        <v>85.78</v>
+      </c>
+      <c r="F57" t="n">
+        <v>55.78</v>
+      </c>
+      <c r="G57" t="n">
+        <v>11.45</v>
+      </c>
+      <c r="H57" t="n">
+        <v>82.37</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:55:05</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>88.7</v>
+      </c>
+      <c r="D58" t="n">
+        <v>86.44</v>
+      </c>
+      <c r="E58" t="n">
+        <v>85.92</v>
+      </c>
+      <c r="F58" t="n">
+        <v>54.29</v>
+      </c>
+      <c r="G58" t="n">
+        <v>11.56</v>
+      </c>
+      <c r="H58" t="n">
+        <v>82.37</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:55:30</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>88.59999999999999</v>
+      </c>
+      <c r="D59" t="n">
+        <v>86.42</v>
+      </c>
+      <c r="E59" t="n">
+        <v>85.91</v>
+      </c>
+      <c r="F59" t="n">
+        <v>54.19</v>
+      </c>
+      <c r="G59" t="n">
+        <v>11.56</v>
+      </c>
+      <c r="H59" t="n">
+        <v>82.38</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:55:55</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>89.34999999999999</v>
+      </c>
+      <c r="D60" t="n">
+        <v>86.56999999999999</v>
+      </c>
+      <c r="E60" t="n">
+        <v>85.95</v>
+      </c>
+      <c r="F60" t="n">
+        <v>54.93</v>
+      </c>
+      <c r="G60" t="n">
+        <v>11.56</v>
+      </c>
+      <c r="H60" t="n">
+        <v>82.39</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:56:20</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>89.09999999999999</v>
+      </c>
+      <c r="D61" t="n">
+        <v>87.14</v>
+      </c>
+      <c r="E61" t="n">
+        <v>86.28</v>
+      </c>
+      <c r="F61" t="n">
+        <v>54.5</v>
+      </c>
+      <c r="G61" t="n">
+        <v>11.69</v>
+      </c>
+      <c r="H61" t="n">
+        <v>82.40000000000001</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:56:44</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>88.34999999999999</v>
+      </c>
+      <c r="D62" t="n">
+        <v>86.98999999999999</v>
+      </c>
+      <c r="E62" t="n">
+        <v>86.25</v>
+      </c>
+      <c r="F62" t="n">
+        <v>53.59</v>
+      </c>
+      <c r="G62" t="n">
+        <v>11.53</v>
+      </c>
+      <c r="H62" t="n">
+        <v>82.41</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:57:10</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550CE</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>87.25</v>
+      </c>
+      <c r="D63" t="n">
+        <v>89.2</v>
+      </c>
+      <c r="E63" t="n">
+        <v>91.88</v>
+      </c>
+      <c r="F63" t="n">
+        <v>42.48</v>
+      </c>
+      <c r="G63" t="n">
+        <v>17.29</v>
+      </c>
+      <c r="H63" t="n">
+        <v>104.96</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:59:03</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>94.8</v>
+      </c>
+      <c r="D64" t="n">
+        <v>90.09</v>
+      </c>
+      <c r="E64" t="n">
+        <v>87.43000000000001</v>
+      </c>
+      <c r="F64" t="n">
+        <v>60.42</v>
+      </c>
+      <c r="G64" t="n">
+        <v>12.86</v>
+      </c>
+      <c r="H64" t="n">
+        <v>82.52</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:59:28</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>94.15000000000001</v>
+      </c>
+      <c r="D65" t="n">
+        <v>89.95999999999999</v>
+      </c>
+      <c r="E65" t="n">
+        <v>87.40000000000001</v>
+      </c>
+      <c r="F65" t="n">
+        <v>59.66</v>
+      </c>
+      <c r="G65" t="n">
+        <v>12.94</v>
+      </c>
+      <c r="H65" t="n">
+        <v>82.55</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2026-01-12 10:59:53</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>94.05</v>
+      </c>
+      <c r="D66" t="n">
+        <v>89.94</v>
+      </c>
+      <c r="E66" t="n">
+        <v>87.39</v>
+      </c>
+      <c r="F66" t="n">
+        <v>59.52</v>
+      </c>
+      <c r="G66" t="n">
+        <v>12.94</v>
+      </c>
+      <c r="H66" t="n">
+        <v>82.56999999999999</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:00:47</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>94.59999999999999</v>
+      </c>
+      <c r="D67" t="n">
+        <v>90.90000000000001</v>
+      </c>
+      <c r="E67" t="n">
+        <v>88.04000000000001</v>
+      </c>
+      <c r="F67" t="n">
+        <v>60.18</v>
+      </c>
+      <c r="G67" t="n">
+        <v>13.92</v>
+      </c>
+      <c r="H67" t="n">
+        <v>82.64</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:01:41</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550CE</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>81.34999999999999</v>
+      </c>
+      <c r="D68" t="n">
+        <v>84.64</v>
+      </c>
+      <c r="E68" t="n">
+        <v>88.89</v>
+      </c>
+      <c r="F68" t="n">
+        <v>38.25</v>
+      </c>
+      <c r="G68" t="n">
+        <v>21.09</v>
+      </c>
+      <c r="H68" t="n">
+        <v>104.11</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:02:06</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>95.55</v>
+      </c>
+      <c r="D69" t="n">
+        <v>92.26000000000001</v>
+      </c>
+      <c r="E69" t="n">
+        <v>88.93000000000001</v>
+      </c>
+      <c r="F69" t="n">
+        <v>60.09</v>
+      </c>
+      <c r="G69" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="H69" t="n">
+        <v>82.72</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:02:31</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>96.5</v>
+      </c>
+      <c r="D70" t="n">
+        <v>92.45</v>
+      </c>
+      <c r="E70" t="n">
+        <v>88.98</v>
+      </c>
+      <c r="F70" t="n">
+        <v>61.17</v>
+      </c>
+      <c r="G70" t="n">
+        <v>16.03</v>
+      </c>
+      <c r="H70" t="n">
+        <v>82.75</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:02:57</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>112.95</v>
+      </c>
+      <c r="D71" t="n">
+        <v>115.45</v>
+      </c>
+      <c r="E71" t="n">
+        <v>120.53</v>
+      </c>
+      <c r="F71" t="n">
+        <v>39.51</v>
+      </c>
+      <c r="G71" t="n">
+        <v>21.48</v>
+      </c>
+      <c r="H71" t="n">
+        <v>138.19</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:05:52</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>97.09999999999999</v>
+      </c>
+      <c r="D72" t="n">
+        <v>93.64</v>
+      </c>
+      <c r="E72" t="n">
+        <v>90.2</v>
+      </c>
+      <c r="F72" t="n">
+        <v>61.53</v>
+      </c>
+      <c r="G72" t="n">
+        <v>17.41</v>
+      </c>
+      <c r="H72" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:08:16</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>111.55</v>
+      </c>
+      <c r="D73" t="n">
+        <v>111.92</v>
+      </c>
+      <c r="E73" t="n">
+        <v>116.92</v>
+      </c>
+      <c r="F73" t="n">
+        <v>40.84</v>
+      </c>
+      <c r="G73" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="H73" t="n">
+        <v>137.07</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:08:41</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550CE</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>83.09999999999999</v>
+      </c>
+      <c r="D74" t="n">
+        <v>81.33</v>
+      </c>
+      <c r="E74" t="n">
+        <v>85.23999999999999</v>
+      </c>
+      <c r="F74" t="n">
+        <v>44.91</v>
+      </c>
+      <c r="G74" t="n">
+        <v>25</v>
+      </c>
+      <c r="H74" t="n">
+        <v>102.73</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:09:35</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>111.7</v>
+      </c>
+      <c r="D75" t="n">
+        <v>111.94</v>
+      </c>
+      <c r="E75" t="n">
+        <v>116.06</v>
+      </c>
+      <c r="F75" t="n">
+        <v>41.16</v>
+      </c>
+      <c r="G75" t="n">
+        <v>23.53</v>
+      </c>
+      <c r="H75" t="n">
+        <v>136.73</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:10:01</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>96.59999999999999</v>
+      </c>
+      <c r="D76" t="n">
+        <v>95.04000000000001</v>
+      </c>
+      <c r="E76" t="n">
+        <v>92.28</v>
+      </c>
+      <c r="F76" t="n">
+        <v>58.79</v>
+      </c>
+      <c r="G76" t="n">
+        <v>16.37</v>
+      </c>
+      <c r="H76" t="n">
+        <v>83.22</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:10:56</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>112.7</v>
+      </c>
+      <c r="D77" t="n">
+        <v>111.62</v>
+      </c>
+      <c r="E77" t="n">
+        <v>114.8</v>
+      </c>
+      <c r="F77" t="n">
+        <v>44.06</v>
+      </c>
+      <c r="G77" t="n">
+        <v>23.07</v>
+      </c>
+      <c r="H77" t="n">
+        <v>136.56</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:11:21</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>94.55</v>
+      </c>
+      <c r="D78" t="n">
+        <v>94.37</v>
+      </c>
+      <c r="E78" t="n">
+        <v>92.78</v>
+      </c>
+      <c r="F78" t="n">
+        <v>54.88</v>
+      </c>
+      <c r="G78" t="n">
+        <v>15.23</v>
+      </c>
+      <c r="H78" t="n">
+        <v>83.26000000000001</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:12:46</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>108.5</v>
+      </c>
+      <c r="D79" t="n">
+        <v>110.18</v>
+      </c>
+      <c r="E79" t="n">
+        <v>113</v>
+      </c>
+      <c r="F79" t="n">
+        <v>40.29</v>
+      </c>
+      <c r="G79" t="n">
+        <v>23.28</v>
+      </c>
+      <c r="H79" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:13:11</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>96</v>
+      </c>
+      <c r="D80" t="n">
+        <v>95.23</v>
+      </c>
+      <c r="E80" t="n">
+        <v>93.8</v>
+      </c>
+      <c r="F80" t="n">
+        <v>55.61</v>
+      </c>
+      <c r="G80" t="n">
+        <v>15.78</v>
+      </c>
+      <c r="H80" t="n">
+        <v>83.39</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:13:36</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>99.34999999999999</v>
+      </c>
+      <c r="D81" t="n">
+        <v>95.90000000000001</v>
+      </c>
+      <c r="E81" t="n">
+        <v>93.97</v>
+      </c>
+      <c r="F81" t="n">
+        <v>59.42</v>
+      </c>
+      <c r="G81" t="n">
+        <v>15.78</v>
+      </c>
+      <c r="H81" t="n">
+        <v>83.41</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:15:31</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>110.25</v>
+      </c>
+      <c r="D82" t="n">
+        <v>99.45999999999999</v>
+      </c>
+      <c r="E82" t="n">
+        <v>95.59</v>
+      </c>
+      <c r="F82" t="n">
+        <v>69.29000000000001</v>
+      </c>
+      <c r="G82" t="n">
+        <v>18.26</v>
+      </c>
+      <c r="H82" t="n">
+        <v>84.31</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:16:26</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>105.65</v>
+      </c>
+      <c r="D83" t="n">
+        <v>99.72</v>
+      </c>
+      <c r="E83" t="n">
+        <v>96.11</v>
+      </c>
+      <c r="F83" t="n">
+        <v>65.84999999999999</v>
+      </c>
+      <c r="G83" t="n">
+        <v>20.39</v>
+      </c>
+      <c r="H83" t="n">
+        <v>85.15000000000001</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:16:46</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>78.75</v>
+      </c>
+      <c r="D84" t="n">
+        <v>73.38</v>
+      </c>
+      <c r="E84" t="n">
+        <v>70.51000000000001</v>
+      </c>
+      <c r="F84" t="n">
+        <v>65.89</v>
+      </c>
+      <c r="G84" t="n">
+        <v>19.6</v>
+      </c>
+      <c r="H84" t="n">
+        <v>64.48</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:17:12</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>109.9</v>
+      </c>
+      <c r="D85" t="n">
+        <v>102.07</v>
+      </c>
+      <c r="E85" t="n">
+        <v>97.25</v>
+      </c>
+      <c r="F85" t="n">
+        <v>69.48999999999999</v>
+      </c>
+      <c r="G85" t="n">
+        <v>22.42</v>
+      </c>
+      <c r="H85" t="n">
+        <v>85.73</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:17:32</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600PE</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>115.15</v>
+      </c>
+      <c r="D86" t="n">
+        <v>103.12</v>
+      </c>
+      <c r="E86" t="n">
+        <v>97.51000000000001</v>
+      </c>
+      <c r="F86" t="n">
+        <v>73.14</v>
+      </c>
+      <c r="G86" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="H86" t="n">
+        <v>85.84999999999999</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:17:53</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>88.8</v>
+      </c>
+      <c r="D87" t="n">
+        <v>76.61</v>
+      </c>
+      <c r="E87" t="n">
+        <v>71.73999999999999</v>
+      </c>
+      <c r="F87" t="n">
+        <v>74.62</v>
+      </c>
+      <c r="G87" t="n">
+        <v>22.53</v>
+      </c>
+      <c r="H87" t="n">
+        <v>65.12</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:18:13</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>85.40000000000001</v>
+      </c>
+      <c r="D88" t="n">
+        <v>78.06999999999999</v>
+      </c>
+      <c r="E88" t="n">
+        <v>72.45</v>
+      </c>
+      <c r="F88" t="n">
+        <v>70.2</v>
+      </c>
+      <c r="G88" t="n">
+        <v>25.33</v>
+      </c>
+      <c r="H88" t="n">
+        <v>65.44</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:18:33</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>83.34999999999999</v>
+      </c>
+      <c r="D89" t="n">
+        <v>77.66</v>
+      </c>
+      <c r="E89" t="n">
+        <v>72.34</v>
+      </c>
+      <c r="F89" t="n">
+        <v>66.43000000000001</v>
+      </c>
+      <c r="G89" t="n">
+        <v>25.33</v>
+      </c>
+      <c r="H89" t="n">
+        <v>65.48999999999999</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:19:23</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="D90" t="n">
+        <v>78.95999999999999</v>
+      </c>
+      <c r="E90" t="n">
+        <v>73.09</v>
+      </c>
+      <c r="F90" t="n">
+        <v>67.08</v>
+      </c>
+      <c r="G90" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="H90" t="n">
+        <v>65.73999999999999</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:19:43</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>86.25</v>
+      </c>
+      <c r="D91" t="n">
+        <v>79.23</v>
+      </c>
+      <c r="E91" t="n">
+        <v>73.16</v>
+      </c>
+      <c r="F91" t="n">
+        <v>68.19</v>
+      </c>
+      <c r="G91" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="H91" t="n">
+        <v>65.79000000000001</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:23:31</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>87.90000000000001</v>
+      </c>
+      <c r="D92" t="n">
+        <v>83.68000000000001</v>
+      </c>
+      <c r="E92" t="n">
+        <v>76.65000000000001</v>
+      </c>
+      <c r="F92" t="n">
+        <v>67.61</v>
+      </c>
+      <c r="G92" t="n">
+        <v>37.45</v>
+      </c>
+      <c r="H92" t="n">
+        <v>66.98</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:24:21</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>89.3</v>
+      </c>
+      <c r="D93" t="n">
+        <v>92.54000000000001</v>
+      </c>
+      <c r="E93" t="n">
+        <v>100.57</v>
+      </c>
+      <c r="F93" t="n">
+        <v>32.94</v>
+      </c>
+      <c r="G93" t="n">
+        <v>43.59</v>
+      </c>
+      <c r="H93" t="n">
+        <v>127.59</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:25:16</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>87.05</v>
+      </c>
+      <c r="D94" t="n">
+        <v>84.94</v>
+      </c>
+      <c r="E94" t="n">
+        <v>78.31999999999999</v>
+      </c>
+      <c r="F94" t="n">
+        <v>64.95</v>
+      </c>
+      <c r="G94" t="n">
+        <v>41.38</v>
+      </c>
+      <c r="H94" t="n">
+        <v>67.27</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:26:06</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>90.40000000000001</v>
+      </c>
+      <c r="D95" t="n">
+        <v>91.89</v>
+      </c>
+      <c r="E95" t="n">
+        <v>98.81999999999999</v>
+      </c>
+      <c r="F95" t="n">
+        <v>35.02</v>
+      </c>
+      <c r="G95" t="n">
+        <v>45.73</v>
+      </c>
+      <c r="H95" t="n">
+        <v>126.75</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:26:30</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>90.59999999999999</v>
+      </c>
+      <c r="D96" t="n">
+        <v>91.93000000000001</v>
+      </c>
+      <c r="E96" t="n">
+        <v>98.84</v>
+      </c>
+      <c r="F96" t="n">
+        <v>35.2</v>
+      </c>
+      <c r="G96" t="n">
+        <v>45.71</v>
+      </c>
+      <c r="H96" t="n">
+        <v>126.54</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:27:25</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>91.45</v>
+      </c>
+      <c r="D97" t="n">
+        <v>91.72</v>
+      </c>
+      <c r="E97" t="n">
+        <v>97.81</v>
+      </c>
+      <c r="F97" t="n">
+        <v>37.29</v>
+      </c>
+      <c r="G97" t="n">
+        <v>46.02</v>
+      </c>
+      <c r="H97" t="n">
+        <v>126.1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:27:51</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>89.8</v>
+      </c>
+      <c r="D98" t="n">
+        <v>91.39</v>
+      </c>
+      <c r="E98" t="n">
+        <v>97.73</v>
+      </c>
+      <c r="F98" t="n">
+        <v>34.46</v>
+      </c>
+      <c r="G98" t="n">
+        <v>46.02</v>
+      </c>
+      <c r="H98" t="n">
+        <v>125.9</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:28:15</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>91.40000000000001</v>
+      </c>
+      <c r="D99" t="n">
+        <v>91.33</v>
+      </c>
+      <c r="E99" t="n">
+        <v>96.68000000000001</v>
+      </c>
+      <c r="F99" t="n">
+        <v>37.79</v>
+      </c>
+      <c r="G99" t="n">
+        <v>46.33</v>
+      </c>
+      <c r="H99" t="n">
+        <v>125.7</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:29:39</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>89</v>
+      </c>
+      <c r="D100" t="n">
+        <v>85.84</v>
+      </c>
+      <c r="E100" t="n">
+        <v>81.58</v>
+      </c>
+      <c r="F100" t="n">
+        <v>66.11</v>
+      </c>
+      <c r="G100" t="n">
+        <v>41.12</v>
+      </c>
+      <c r="H100" t="n">
+        <v>67.2</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:31:29</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>93.65000000000001</v>
+      </c>
+      <c r="D101" t="n">
+        <v>88.43000000000001</v>
+      </c>
+      <c r="E101" t="n">
+        <v>83.89</v>
+      </c>
+      <c r="F101" t="n">
+        <v>70.98999999999999</v>
+      </c>
+      <c r="G101" t="n">
+        <v>43.74</v>
+      </c>
+      <c r="H101" t="n">
+        <v>67.86</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:31:49</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>93.15000000000001</v>
+      </c>
+      <c r="D102" t="n">
+        <v>88.33</v>
+      </c>
+      <c r="E102" t="n">
+        <v>83.87</v>
+      </c>
+      <c r="F102" t="n">
+        <v>70.51000000000001</v>
+      </c>
+      <c r="G102" t="n">
+        <v>43.74</v>
+      </c>
+      <c r="H102" t="n">
+        <v>67.91</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:32:39</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>103.55</v>
+      </c>
+      <c r="D103" t="n">
+        <v>91.86</v>
+      </c>
+      <c r="E103" t="n">
+        <v>85.72</v>
+      </c>
+      <c r="F103" t="n">
+        <v>78.38</v>
+      </c>
+      <c r="G103" t="n">
+        <v>45.58</v>
+      </c>
+      <c r="H103" t="n">
+        <v>68.27</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:33:35</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500PE</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>76.84999999999999</v>
+      </c>
+      <c r="D104" t="n">
+        <v>68.56999999999999</v>
+      </c>
+      <c r="E104" t="n">
+        <v>63.38</v>
+      </c>
+      <c r="F104" t="n">
+        <v>78.61</v>
+      </c>
+      <c r="G104" t="n">
+        <v>46.05</v>
+      </c>
+      <c r="H104" t="n">
+        <v>51.84</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:34:00</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>104.75</v>
+      </c>
+      <c r="D105" t="n">
+        <v>93.84999999999999</v>
+      </c>
+      <c r="E105" t="n">
+        <v>87.09999999999999</v>
+      </c>
+      <c r="F105" t="n">
+        <v>79.23999999999999</v>
+      </c>
+      <c r="G105" t="n">
+        <v>47.61</v>
+      </c>
+      <c r="H105" t="n">
+        <v>68.84</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:35:55</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>109.55</v>
+      </c>
+      <c r="D106" t="n">
+        <v>111.12</v>
+      </c>
+      <c r="E106" t="n">
+        <v>118.36</v>
+      </c>
+      <c r="F106" t="n">
+        <v>34.08</v>
+      </c>
+      <c r="G106" t="n">
+        <v>54.98</v>
+      </c>
+      <c r="H106" t="n">
+        <v>147.49</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:36:20</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>80.40000000000001</v>
+      </c>
+      <c r="D107" t="n">
+        <v>80.87</v>
+      </c>
+      <c r="E107" t="n">
+        <v>86.14</v>
+      </c>
+      <c r="F107" t="n">
+        <v>35.05</v>
+      </c>
+      <c r="G107" t="n">
+        <v>53.68</v>
+      </c>
+      <c r="H107" t="n">
+        <v>115.65</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:36:44</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>80.15000000000001</v>
+      </c>
+      <c r="D108" t="n">
+        <v>80.81999999999999</v>
+      </c>
+      <c r="E108" t="n">
+        <v>86.13</v>
+      </c>
+      <c r="F108" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="G108" t="n">
+        <v>53.33</v>
+      </c>
+      <c r="H108" t="n">
+        <v>115.28</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:37:09</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>108.45</v>
+      </c>
+      <c r="D109" t="n">
+        <v>110.27</v>
+      </c>
+      <c r="E109" t="n">
+        <v>116.55</v>
+      </c>
+      <c r="F109" t="n">
+        <v>33.42</v>
+      </c>
+      <c r="G109" t="n">
+        <v>52.94</v>
+      </c>
+      <c r="H109" t="n">
+        <v>145.23</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:37:34</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>106.8</v>
+      </c>
+      <c r="D110" t="n">
+        <v>109.94</v>
+      </c>
+      <c r="E110" t="n">
+        <v>116.46</v>
+      </c>
+      <c r="F110" t="n">
+        <v>32.13</v>
+      </c>
+      <c r="G110" t="n">
+        <v>53.09</v>
+      </c>
+      <c r="H110" t="n">
+        <v>144.85</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:37:59</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>107.15</v>
+      </c>
+      <c r="D111" t="n">
+        <v>110.01</v>
+      </c>
+      <c r="E111" t="n">
+        <v>116.48</v>
+      </c>
+      <c r="F111" t="n">
+        <v>32.39</v>
+      </c>
+      <c r="G111" t="n">
+        <v>53.18</v>
+      </c>
+      <c r="H111" t="n">
+        <v>144.58</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:39:23</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>99.45</v>
+      </c>
+      <c r="D112" t="n">
+        <v>98.29000000000001</v>
+      </c>
+      <c r="E112" t="n">
+        <v>93.03</v>
+      </c>
+      <c r="F112" t="n">
+        <v>64.7</v>
+      </c>
+      <c r="G112" t="n">
+        <v>43.74</v>
+      </c>
+      <c r="H112" t="n">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:39:45</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>101.45</v>
+      </c>
+      <c r="D113" t="n">
+        <v>98.69</v>
+      </c>
+      <c r="E113" t="n">
+        <v>93.13</v>
+      </c>
+      <c r="F113" t="n">
+        <v>67.41</v>
+      </c>
+      <c r="G113" t="n">
+        <v>43.74</v>
+      </c>
+      <c r="H113" t="n">
+        <v>70.52</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:41:05</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>107</v>
+      </c>
+      <c r="D114" t="n">
+        <v>107.98</v>
+      </c>
+      <c r="E114" t="n">
+        <v>112.91</v>
+      </c>
+      <c r="F114" t="n">
+        <v>33.65</v>
+      </c>
+      <c r="G114" t="n">
+        <v>50.29</v>
+      </c>
+      <c r="H114" t="n">
+        <v>141.71</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:41:59</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>106.85</v>
+      </c>
+      <c r="D115" t="n">
+        <v>107.95</v>
+      </c>
+      <c r="E115" t="n">
+        <v>112.9</v>
+      </c>
+      <c r="F115" t="n">
+        <v>33.35</v>
+      </c>
+      <c r="G115" t="n">
+        <v>50.32</v>
+      </c>
+      <c r="H115" t="n">
+        <v>141.26</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:42:24</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>102</v>
+      </c>
+      <c r="D116" t="n">
+        <v>99.68000000000001</v>
+      </c>
+      <c r="E116" t="n">
+        <v>95.22</v>
+      </c>
+      <c r="F116" t="n">
+        <v>66.54000000000001</v>
+      </c>
+      <c r="G116" t="n">
+        <v>40.52</v>
+      </c>
+      <c r="H116" t="n">
+        <v>70.90000000000001</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:42:44</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>101.5</v>
+      </c>
+      <c r="D117" t="n">
+        <v>99.58</v>
+      </c>
+      <c r="E117" t="n">
+        <v>95.2</v>
+      </c>
+      <c r="F117" t="n">
+        <v>66</v>
+      </c>
+      <c r="G117" t="n">
+        <v>40.63</v>
+      </c>
+      <c r="H117" t="n">
+        <v>70.95</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:44:33</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500PE</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>77.45</v>
+      </c>
+      <c r="D118" t="n">
+        <v>74.84</v>
+      </c>
+      <c r="E118" t="n">
+        <v>71.16</v>
+      </c>
+      <c r="F118" t="n">
+        <v>67.38</v>
+      </c>
+      <c r="G118" t="n">
+        <v>39.52</v>
+      </c>
+      <c r="H118" t="n">
+        <v>55.08</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:46:25</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>107.4</v>
+      </c>
+      <c r="D119" t="n">
+        <v>103.74</v>
+      </c>
+      <c r="E119" t="n">
+        <v>99.22</v>
+      </c>
+      <c r="F119" t="n">
+        <v>69.37</v>
+      </c>
+      <c r="G119" t="n">
+        <v>40.97</v>
+      </c>
+      <c r="H119" t="n">
+        <v>71.62</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:47:14</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>78.55</v>
+      </c>
+      <c r="D120" t="n">
+        <v>76.39</v>
+      </c>
+      <c r="E120" t="n">
+        <v>77.97</v>
+      </c>
+      <c r="F120" t="n">
+        <v>42.94</v>
+      </c>
+      <c r="G120" t="n">
+        <v>48.79</v>
+      </c>
+      <c r="H120" t="n">
+        <v>107.23</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:48:40</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>79</v>
+      </c>
+      <c r="D121" t="n">
+        <v>77.36</v>
+      </c>
+      <c r="E121" t="n">
+        <v>77.58</v>
+      </c>
+      <c r="F121" t="n">
+        <v>44.46</v>
+      </c>
+      <c r="G121" t="n">
+        <v>45.75</v>
+      </c>
+      <c r="H121" t="n">
+        <v>106.11</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:49:05</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="D122" t="n">
+        <v>101.04</v>
+      </c>
+      <c r="E122" t="n">
+        <v>100.72</v>
+      </c>
+      <c r="F122" t="n">
+        <v>56.91</v>
+      </c>
+      <c r="G122" t="n">
+        <v>33.63</v>
+      </c>
+      <c r="H122" t="n">
+        <v>72.36</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:49:25</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>108.3</v>
+      </c>
+      <c r="D123" t="n">
+        <v>107.07</v>
+      </c>
+      <c r="E123" t="n">
+        <v>106.84</v>
+      </c>
+      <c r="F123" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="G123" t="n">
+        <v>42.55</v>
+      </c>
+      <c r="H123" t="n">
+        <v>133.56</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:50:51</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>100.35</v>
+      </c>
+      <c r="D124" t="n">
+        <v>100.53</v>
+      </c>
+      <c r="E124" t="n">
+        <v>101.02</v>
+      </c>
+      <c r="F124" t="n">
+        <v>55.27</v>
+      </c>
+      <c r="G124" t="n">
+        <v>31.38</v>
+      </c>
+      <c r="H124" t="n">
+        <v>72.73</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:51:46</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>106.6</v>
+      </c>
+      <c r="D125" t="n">
+        <v>107.37</v>
+      </c>
+      <c r="E125" t="n">
+        <v>106.49</v>
+      </c>
+      <c r="F125" t="n">
+        <v>42.54</v>
+      </c>
+      <c r="G125" t="n">
+        <v>37.94</v>
+      </c>
+      <c r="H125" t="n">
+        <v>131.93</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:52:11</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>102.65</v>
+      </c>
+      <c r="D126" t="n">
+        <v>101.03</v>
+      </c>
+      <c r="E126" t="n">
+        <v>101.39</v>
+      </c>
+      <c r="F126" t="n">
+        <v>58.01</v>
+      </c>
+      <c r="G126" t="n">
+        <v>28.12</v>
+      </c>
+      <c r="H126" t="n">
+        <v>73.05</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:52:33</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550PE</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>100.15</v>
+      </c>
+      <c r="D127" t="n">
+        <v>100.53</v>
+      </c>
+      <c r="E127" t="n">
+        <v>101.27</v>
+      </c>
+      <c r="F127" t="n">
+        <v>54.6</v>
+      </c>
+      <c r="G127" t="n">
+        <v>28.16</v>
+      </c>
+      <c r="H127" t="n">
+        <v>73.09</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:53:27</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>109.35</v>
+      </c>
+      <c r="D128" t="n">
+        <v>108</v>
+      </c>
+      <c r="E128" t="n">
+        <v>106.78</v>
+      </c>
+      <c r="F128" t="n">
+        <v>46.89</v>
+      </c>
+      <c r="G128" t="n">
+        <v>34.68</v>
+      </c>
+      <c r="H128" t="n">
+        <v>130.99</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:54:21</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>109.05</v>
+      </c>
+      <c r="D129" t="n">
+        <v>108.24</v>
+      </c>
+      <c r="E129" t="n">
+        <v>107.11</v>
+      </c>
+      <c r="F129" t="n">
+        <v>46.49</v>
+      </c>
+      <c r="G129" t="n">
+        <v>32.86</v>
+      </c>
+      <c r="H129" t="n">
+        <v>130.6</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:54:46</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>108.7</v>
+      </c>
+      <c r="D130" t="n">
+        <v>108.17</v>
+      </c>
+      <c r="E130" t="n">
+        <v>107.1</v>
+      </c>
+      <c r="F130" t="n">
+        <v>46.01</v>
+      </c>
+      <c r="G130" t="n">
+        <v>32.86</v>
+      </c>
+      <c r="H130" t="n">
+        <v>130.56</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:55:11</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>109.75</v>
+      </c>
+      <c r="D131" t="n">
+        <v>108.49</v>
+      </c>
+      <c r="E131" t="n">
+        <v>107.09</v>
+      </c>
+      <c r="F131" t="n">
+        <v>47.75</v>
+      </c>
+      <c r="G131" t="n">
+        <v>31.14</v>
+      </c>
+      <c r="H131" t="n">
+        <v>130.26</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:56:35</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>109.45</v>
+      </c>
+      <c r="D132" t="n">
+        <v>108.72</v>
+      </c>
+      <c r="E132" t="n">
+        <v>107.13</v>
+      </c>
+      <c r="F132" t="n">
+        <v>47.29</v>
+      </c>
+      <c r="G132" t="n">
+        <v>28.59</v>
+      </c>
+      <c r="H132" t="n">
+        <v>129.62</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:57:30</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>110.1</v>
+      </c>
+      <c r="D133" t="n">
+        <v>108.92</v>
+      </c>
+      <c r="E133" t="n">
+        <v>107.26</v>
+      </c>
+      <c r="F133" t="n">
+        <v>48.57</v>
+      </c>
+      <c r="G133" t="n">
+        <v>26.74</v>
+      </c>
+      <c r="H133" t="n">
+        <v>129.32</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2026-01-12 11:58:59</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>111.85</v>
+      </c>
+      <c r="D134" t="n">
+        <v>109.55</v>
+      </c>
+      <c r="E134" t="n">
+        <v>107.53</v>
+      </c>
+      <c r="F134" t="n">
+        <v>51.59</v>
+      </c>
+      <c r="G134" t="n">
+        <v>25.21</v>
+      </c>
+      <c r="H134" t="n">
+        <v>128.91</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:01:24</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>82.34999999999999</v>
+      </c>
+      <c r="D135" t="n">
+        <v>80.14</v>
+      </c>
+      <c r="E135" t="n">
+        <v>78.25</v>
+      </c>
+      <c r="F135" t="n">
+        <v>53.96</v>
+      </c>
+      <c r="G135" t="n">
+        <v>23.44</v>
+      </c>
+      <c r="H135" t="n">
+        <v>99.47</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:02:50</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>NIFTY2611325450CE</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>115.6</v>
+      </c>
+      <c r="D136" t="n">
+        <v>111.96</v>
+      </c>
+      <c r="E136" t="n">
+        <v>108.92</v>
+      </c>
+      <c r="F136" t="n">
+        <v>57.6</v>
+      </c>
+      <c r="G136" t="n">
+        <v>23.09</v>
+      </c>
+      <c r="H136" t="n">
+        <v>127.48</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:06:51</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="D137" t="n">
+        <v>81.79000000000001</v>
+      </c>
+      <c r="E137" t="n">
+        <v>80.25</v>
+      </c>
+      <c r="F137" t="n">
+        <v>55.12</v>
+      </c>
+      <c r="G137" t="n">
+        <v>22.55</v>
+      </c>
+      <c r="H137" t="n">
+        <v>97.08</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:07:16</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>84.25</v>
+      </c>
+      <c r="D138" t="n">
+        <v>82.19</v>
+      </c>
+      <c r="E138" t="n">
+        <v>80.36</v>
+      </c>
+      <c r="F138" t="n">
+        <v>56.32</v>
+      </c>
+      <c r="G138" t="n">
+        <v>22.85</v>
+      </c>
+      <c r="H138" t="n">
+        <v>96.81999999999999</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:07:41</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="D139" t="n">
+        <v>82.40000000000001</v>
+      </c>
+      <c r="E139" t="n">
+        <v>80.42</v>
+      </c>
+      <c r="F139" t="n">
+        <v>58.15</v>
+      </c>
+      <c r="G139" t="n">
+        <v>23.27</v>
+      </c>
+      <c r="H139" t="n">
+        <v>96.70999999999999</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:08:38</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>90.5</v>
+      </c>
+      <c r="D140" t="n">
+        <v>84.23999999999999</v>
+      </c>
+      <c r="E140" t="n">
+        <v>81.15000000000001</v>
+      </c>
+      <c r="F140" t="n">
+        <v>65.68000000000001</v>
+      </c>
+      <c r="G140" t="n">
+        <v>25.72</v>
+      </c>
+      <c r="H140" t="n">
+        <v>96.37</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:10:35</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>93.55</v>
+      </c>
+      <c r="D141" t="n">
+        <v>86.69</v>
+      </c>
+      <c r="E141" t="n">
+        <v>82.31</v>
+      </c>
+      <c r="F141" t="n">
+        <v>69.72</v>
+      </c>
+      <c r="G141" t="n">
+        <v>30.46</v>
+      </c>
+      <c r="H141" t="n">
+        <v>95.72</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:13:01</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>93.3</v>
+      </c>
+      <c r="D142" t="n">
+        <v>89.14</v>
+      </c>
+      <c r="E142" t="n">
+        <v>84.25</v>
+      </c>
+      <c r="F142" t="n">
+        <v>66.94</v>
+      </c>
+      <c r="G142" t="n">
+        <v>34.92</v>
+      </c>
+      <c r="H142" t="n">
+        <v>95.12</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:13:26</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>96.25</v>
+      </c>
+      <c r="D143" t="n">
+        <v>89.73</v>
+      </c>
+      <c r="E143" t="n">
+        <v>84.40000000000001</v>
+      </c>
+      <c r="F143" t="n">
+        <v>70.25</v>
+      </c>
+      <c r="G143" t="n">
+        <v>35.35</v>
+      </c>
+      <c r="H143" t="n">
+        <v>95.13</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:13:47</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>104.1</v>
+      </c>
+      <c r="D144" t="n">
+        <v>91.3</v>
+      </c>
+      <c r="E144" t="n">
+        <v>84.79000000000001</v>
+      </c>
+      <c r="F144" t="n">
+        <v>76.53</v>
+      </c>
+      <c r="G144" t="n">
+        <v>36.1</v>
+      </c>
+      <c r="H144" t="n">
+        <v>95.39</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:14:12</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>NIFTY2611325500CE</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>106.35</v>
+      </c>
+      <c r="D145" t="n">
+        <v>94.09</v>
+      </c>
+      <c r="E145" t="n">
+        <v>86.09999999999999</v>
+      </c>
+      <c r="F145" t="n">
+        <v>78.02</v>
+      </c>
+      <c r="G145" t="n">
+        <v>38.77</v>
+      </c>
+      <c r="H145" t="n">
+        <v>95.34</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:16:10</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550CE</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>93.75</v>
+      </c>
+      <c r="D146" t="n">
+        <v>81.2</v>
+      </c>
+      <c r="E146" t="n">
+        <v>66.20999999999999</v>
+      </c>
+      <c r="F146" t="n">
+        <v>74.05</v>
+      </c>
+      <c r="G146" t="n">
+        <v>46.37</v>
+      </c>
+      <c r="H146" t="n">
+        <v>75.34</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:16:30</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550CE</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>103.1</v>
+      </c>
+      <c r="D147" t="n">
+        <v>83.06999999999999</v>
+      </c>
+      <c r="E147" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="F147" t="n">
+        <v>84.98</v>
+      </c>
+      <c r="G147" t="n">
+        <v>46.37</v>
+      </c>
+      <c r="H147" t="n">
+        <v>75.68000000000001</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:17:27</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>NIFTY2611325550CE</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>112.25</v>
+      </c>
+      <c r="D148" t="n">
+        <v>89.31999999999999</v>
+      </c>
+      <c r="E148" t="n">
+        <v>69.64</v>
+      </c>
+      <c r="F148" t="n">
+        <v>87.29000000000001</v>
+      </c>
+      <c r="G148" t="n">
+        <v>48.02</v>
+      </c>
+      <c r="H148" t="n">
+        <v>76.40000000000001</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:18:22</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600CE</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>96.75</v>
+      </c>
+      <c r="D149" t="n">
+        <v>72.8</v>
+      </c>
+      <c r="E149" t="n">
+        <v>52.22</v>
+      </c>
+      <c r="F149" t="n">
+        <v>90.51000000000001</v>
+      </c>
+      <c r="G149" t="n">
+        <v>50.04</v>
+      </c>
+      <c r="H149" t="n">
+        <v>59.52</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:20:17</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600CE</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>96.05</v>
+      </c>
+      <c r="D150" t="n">
+        <v>79.98</v>
+      </c>
+      <c r="E150" t="n">
+        <v>57.62</v>
+      </c>
+      <c r="F150" t="n">
+        <v>82.7</v>
+      </c>
+      <c r="G150" t="n">
+        <v>52.61</v>
+      </c>
+      <c r="H150" t="n">
+        <v>60.68</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:20:42</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600CE</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>103.8</v>
+      </c>
+      <c r="D151" t="n">
+        <v>81.53</v>
+      </c>
+      <c r="E151" t="n">
+        <v>58.01</v>
+      </c>
+      <c r="F151" t="n">
+        <v>84.69</v>
+      </c>
+      <c r="G151" t="n">
+        <v>52.87</v>
+      </c>
+      <c r="H151" t="n">
+        <v>61.3</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:21:38</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>NIFTY2611325600CE</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>120.5</v>
+      </c>
+      <c r="D152" t="n">
+        <v>89.09</v>
+      </c>
+      <c r="E152" t="n">
+        <v>61.96</v>
+      </c>
+      <c r="F152" t="n">
+        <v>87.93000000000001</v>
+      </c>
+      <c r="G152" t="n">
+        <v>54.72</v>
+      </c>
+      <c r="H152" t="n">
+        <v>62.83</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:22:03</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>NIFTY2611325650CE</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>99.2</v>
+      </c>
+      <c r="D153" t="n">
+        <v>73.45999999999999</v>
+      </c>
+      <c r="E153" t="n">
+        <v>47.64</v>
+      </c>
+      <c r="F153" t="n">
+        <v>85.33</v>
+      </c>
+      <c r="G153" t="n">
+        <v>56.12</v>
+      </c>
+      <c r="H153" t="n">
+        <v>47.46</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:22:58</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>NIFTY2611325650CE</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>85.75</v>
+      </c>
+      <c r="D154" t="n">
+        <v>70.77</v>
+      </c>
+      <c r="E154" t="n">
+        <v>46.97</v>
+      </c>
+      <c r="F154" t="n">
+        <v>72.31</v>
+      </c>
+      <c r="G154" t="n">
+        <v>56.12</v>
+      </c>
+      <c r="H154" t="n">
+        <v>48.81</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:24:19</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700PE</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>99.25</v>
+      </c>
+      <c r="D155" t="n">
+        <v>114.1</v>
+      </c>
+      <c r="E155" t="n">
+        <v>151.14</v>
+      </c>
+      <c r="F155" t="n">
+        <v>27.09</v>
+      </c>
+      <c r="G155" t="n">
+        <v>57.69</v>
+      </c>
+      <c r="H155" t="n">
+        <v>155.47</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:24:43</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700PE</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>103</v>
+      </c>
+      <c r="D156" t="n">
+        <v>114.85</v>
+      </c>
+      <c r="E156" t="n">
+        <v>151.32</v>
+      </c>
+      <c r="F156" t="n">
+        <v>29.26</v>
+      </c>
+      <c r="G156" t="n">
+        <v>57.69</v>
+      </c>
+      <c r="H156" t="n">
+        <v>155.06</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:26:37</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>NIFTY2611325650CE</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>104.1</v>
+      </c>
+      <c r="D157" t="n">
+        <v>87.33</v>
+      </c>
+      <c r="E157" t="n">
+        <v>61.3</v>
+      </c>
+      <c r="F157" t="n">
+        <v>77.98999999999999</v>
+      </c>
+      <c r="G157" t="n">
+        <v>63.37</v>
+      </c>
+      <c r="H157" t="n">
+        <v>52.41</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:28:30</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700PE</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>98.84999999999999</v>
+      </c>
+      <c r="D158" t="n">
+        <v>102.84</v>
+      </c>
+      <c r="E158" t="n">
+        <v>130.42</v>
+      </c>
+      <c r="F158" t="n">
+        <v>32.02</v>
+      </c>
+      <c r="G158" t="n">
+        <v>61.07</v>
+      </c>
+      <c r="H158" t="n">
+        <v>150.57</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:28:57</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700PE</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>102</v>
+      </c>
+      <c r="D159" t="n">
+        <v>103.47</v>
+      </c>
+      <c r="E159" t="n">
+        <v>130.57</v>
+      </c>
+      <c r="F159" t="n">
+        <v>33.85</v>
+      </c>
+      <c r="G159" t="n">
+        <v>60.71</v>
+      </c>
+      <c r="H159" t="n">
+        <v>150.05</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:29:53</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700PE</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>99.34999999999999</v>
+      </c>
+      <c r="D160" t="n">
+        <v>102.6</v>
+      </c>
+      <c r="E160" t="n">
+        <v>125.87</v>
+      </c>
+      <c r="F160" t="n">
+        <v>32.96</v>
+      </c>
+      <c r="G160" t="n">
+        <v>59.89</v>
+      </c>
+      <c r="H160" t="n">
+        <v>148.83</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:31:17</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>84.84999999999999</v>
+      </c>
+      <c r="D161" t="n">
+        <v>75</v>
+      </c>
+      <c r="E161" t="n">
+        <v>58.79</v>
+      </c>
+      <c r="F161" t="n">
+        <v>71.15000000000001</v>
+      </c>
+      <c r="G161" t="n">
+        <v>60.6</v>
+      </c>
+      <c r="H161" t="n">
+        <v>42.63</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:32:07</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>NIFTY2611325650CE</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>111.5</v>
+      </c>
+      <c r="D162" t="n">
+        <v>102.03</v>
+      </c>
+      <c r="E162" t="n">
+        <v>84.45999999999999</v>
+      </c>
+      <c r="F162" t="n">
+        <v>69.13</v>
+      </c>
+      <c r="G162" t="n">
+        <v>63</v>
+      </c>
+      <c r="H162" t="n">
+        <v>57.78</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:32:27</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>NIFTY2611325650CE</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>115.55</v>
+      </c>
+      <c r="D163" t="n">
+        <v>102.84</v>
+      </c>
+      <c r="E163" t="n">
+        <v>84.66</v>
+      </c>
+      <c r="F163" t="n">
+        <v>70.40000000000001</v>
+      </c>
+      <c r="G163" t="n">
+        <v>63.06</v>
+      </c>
+      <c r="H163" t="n">
+        <v>58.05</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:32:47</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>98.65000000000001</v>
+      </c>
+      <c r="D164" t="n">
+        <v>79.12</v>
+      </c>
+      <c r="E164" t="n">
+        <v>62.51</v>
+      </c>
+      <c r="F164" t="n">
+        <v>74.58</v>
+      </c>
+      <c r="G164" t="n">
+        <v>60.76</v>
+      </c>
+      <c r="H164" t="n">
+        <v>44.55</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:33:08</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>91.34999999999999</v>
+      </c>
+      <c r="D165" t="n">
+        <v>80.31999999999999</v>
+      </c>
+      <c r="E165" t="n">
+        <v>65.5</v>
+      </c>
+      <c r="F165" t="n">
+        <v>72.31</v>
+      </c>
+      <c r="G165" t="n">
+        <v>60.88</v>
+      </c>
+      <c r="H165" t="n">
+        <v>45.08</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:33:58</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>100</v>
+      </c>
+      <c r="D166" t="n">
+        <v>82.05</v>
+      </c>
+      <c r="E166" t="n">
+        <v>65.94</v>
+      </c>
+      <c r="F166" t="n">
+        <v>75.16</v>
+      </c>
+      <c r="G166" t="n">
+        <v>60.92</v>
+      </c>
+      <c r="H166" t="n">
+        <v>46.19</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:34:55</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>94.84999999999999</v>
+      </c>
+      <c r="D167" t="n">
+        <v>84.47</v>
+      </c>
+      <c r="E167" t="n">
+        <v>68.79000000000001</v>
+      </c>
+      <c r="F167" t="n">
+        <v>70.95999999999999</v>
+      </c>
+      <c r="G167" t="n">
+        <v>61.06</v>
+      </c>
+      <c r="H167" t="n">
+        <v>47.13</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:36:44</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750PE</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>105.8</v>
+      </c>
+      <c r="D168" t="n">
+        <v>112.7</v>
+      </c>
+      <c r="E168" t="n">
+        <v>125.5</v>
+      </c>
+      <c r="F168" t="n">
+        <v>30.07</v>
+      </c>
+      <c r="G168" t="n">
+        <v>61.29</v>
+      </c>
+      <c r="H168" t="n">
+        <v>172.62</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:37:08</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>96.59999999999999</v>
+      </c>
+      <c r="D169" t="n">
+        <v>89.77</v>
+      </c>
+      <c r="E169" t="n">
+        <v>76.97</v>
+      </c>
+      <c r="F169" t="n">
+        <v>70.22</v>
+      </c>
+      <c r="G169" t="n">
+        <v>59.4</v>
+      </c>
+      <c r="H169" t="n">
+        <v>49.14</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:38:57</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700PE</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>88.8</v>
+      </c>
+      <c r="D170" t="n">
+        <v>85.68000000000001</v>
+      </c>
+      <c r="E170" t="n">
+        <v>92.59999999999999</v>
+      </c>
+      <c r="F170" t="n">
+        <v>37.91</v>
+      </c>
+      <c r="G170" t="n">
+        <v>57.74</v>
+      </c>
+      <c r="H170" t="n">
+        <v>133.17</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:40:23</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750PE</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>112</v>
+      </c>
+      <c r="D171" t="n">
+        <v>112.32</v>
+      </c>
+      <c r="E171" t="n">
+        <v>116.97</v>
+      </c>
+      <c r="F171" t="n">
+        <v>35.69</v>
+      </c>
+      <c r="G171" t="n">
+        <v>57.61</v>
+      </c>
+      <c r="H171" t="n">
+        <v>166.78</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:40:48</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>88.95</v>
+      </c>
+      <c r="D172" t="n">
+        <v>87.2</v>
+      </c>
+      <c r="E172" t="n">
+        <v>82.18000000000001</v>
+      </c>
+      <c r="F172" t="n">
+        <v>62.2</v>
+      </c>
+      <c r="G172" t="n">
+        <v>53.92</v>
+      </c>
+      <c r="H172" t="n">
+        <v>51.27</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:41:38</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>96.2</v>
+      </c>
+      <c r="D173" t="n">
+        <v>88.18000000000001</v>
+      </c>
+      <c r="E173" t="n">
+        <v>82.98</v>
+      </c>
+      <c r="F173" t="n">
+        <v>65.98</v>
+      </c>
+      <c r="G173" t="n">
+        <v>53</v>
+      </c>
+      <c r="H173" t="n">
+        <v>51.93</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:41:58</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>92.8</v>
+      </c>
+      <c r="D174" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="E174" t="n">
+        <v>82.81</v>
+      </c>
+      <c r="F174" t="n">
+        <v>64.39</v>
+      </c>
+      <c r="G174" t="n">
+        <v>53</v>
+      </c>
+      <c r="H174" t="n">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:42:48</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>112.4</v>
+      </c>
+      <c r="D175" t="n">
+        <v>92.54000000000001</v>
+      </c>
+      <c r="E175" t="n">
+        <v>85.22</v>
+      </c>
+      <c r="F175" t="n">
+        <v>72.40000000000001</v>
+      </c>
+      <c r="G175" t="n">
+        <v>53.18</v>
+      </c>
+      <c r="H175" t="n">
+        <v>53.66</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:43:08</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750CE</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>88.05</v>
+      </c>
+      <c r="D176" t="n">
+        <v>73.31</v>
+      </c>
+      <c r="E176" t="n">
+        <v>64.70999999999999</v>
+      </c>
+      <c r="F176" t="n">
+        <v>71.65000000000001</v>
+      </c>
+      <c r="G176" t="n">
+        <v>53.77</v>
+      </c>
+      <c r="H176" t="n">
+        <v>40.23</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:43:29</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750CE</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>90.84999999999999</v>
+      </c>
+      <c r="D177" t="n">
+        <v>73.87</v>
+      </c>
+      <c r="E177" t="n">
+        <v>64.84</v>
+      </c>
+      <c r="F177" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="G177" t="n">
+        <v>53.77</v>
+      </c>
+      <c r="H177" t="n">
+        <v>40.89</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:45:18</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750CE</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>92.8</v>
+      </c>
+      <c r="D178" t="n">
+        <v>78.79000000000001</v>
+      </c>
+      <c r="E178" t="n">
+        <v>68.34</v>
+      </c>
+      <c r="F178" t="n">
+        <v>72.23</v>
+      </c>
+      <c r="G178" t="n">
+        <v>54.07</v>
+      </c>
+      <c r="H178" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:45:38</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750PE</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>86.90000000000001</v>
+      </c>
+      <c r="D179" t="n">
+        <v>96.91</v>
+      </c>
+      <c r="E179" t="n">
+        <v>108.02</v>
+      </c>
+      <c r="F179" t="n">
+        <v>30.99</v>
+      </c>
+      <c r="G179" t="n">
+        <v>57.15</v>
+      </c>
+      <c r="H179" t="n">
+        <v>147.7</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:46:03</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750CE</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>87.84999999999999</v>
+      </c>
+      <c r="D180" t="n">
+        <v>79.76000000000001</v>
+      </c>
+      <c r="E180" t="n">
+        <v>69.68000000000001</v>
+      </c>
+      <c r="F180" t="n">
+        <v>70.23</v>
+      </c>
+      <c r="G180" t="n">
+        <v>54.65</v>
+      </c>
+      <c r="H180" t="n">
+        <v>44.32</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:46:23</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750PE</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
+        <v>93.75</v>
+      </c>
+      <c r="D181" t="n">
+        <v>97.06999999999999</v>
+      </c>
+      <c r="E181" t="n">
+        <v>106.79</v>
+      </c>
+      <c r="F181" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="G181" t="n">
+        <v>56.76</v>
+      </c>
+      <c r="H181" t="n">
+        <v>144.53</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:46:50</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750PE</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>95.84999999999999</v>
+      </c>
+      <c r="D182" t="n">
+        <v>97.48999999999999</v>
+      </c>
+      <c r="E182" t="n">
+        <v>106.9</v>
+      </c>
+      <c r="F182" t="n">
+        <v>35.96</v>
+      </c>
+      <c r="G182" t="n">
+        <v>56.52</v>
+      </c>
+      <c r="H182" t="n">
+        <v>143.91</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:47:45</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750PE</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
+        <v>95.45</v>
+      </c>
+      <c r="D183" t="n">
+        <v>97.41</v>
+      </c>
+      <c r="E183" t="n">
+        <v>105.97</v>
+      </c>
+      <c r="F183" t="n">
+        <v>36.33</v>
+      </c>
+      <c r="G183" t="n">
+        <v>55.55</v>
+      </c>
+      <c r="H183" t="n">
+        <v>141.44</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:48:39</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750PE</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>100.6</v>
+      </c>
+      <c r="D184" t="n">
+        <v>98.22</v>
+      </c>
+      <c r="E184" t="n">
+        <v>104.45</v>
+      </c>
+      <c r="F184" t="n">
+        <v>39.68</v>
+      </c>
+      <c r="G184" t="n">
+        <v>54.31</v>
+      </c>
+      <c r="H184" t="n">
+        <v>140.16</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:49:05</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750CE</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>81.40000000000001</v>
+      </c>
+      <c r="D185" t="n">
+        <v>80.42</v>
+      </c>
+      <c r="E185" t="n">
+        <v>73.42</v>
+      </c>
+      <c r="F185" t="n">
+        <v>62.66</v>
+      </c>
+      <c r="G185" t="n">
+        <v>51.75</v>
+      </c>
+      <c r="H185" t="n">
+        <v>46.43</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:49:55</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>NIFTY2611325750PE</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>99.45</v>
+      </c>
+      <c r="D186" t="n">
+        <v>97.73</v>
+      </c>
+      <c r="E186" t="n">
+        <v>102.82</v>
+      </c>
+      <c r="F186" t="n">
+        <v>39.19</v>
+      </c>
+      <c r="G186" t="n">
+        <v>53.18</v>
+      </c>
+      <c r="H186" t="n">
+        <v>138.8</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:50:50</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
+        <v>113</v>
+      </c>
+      <c r="D187" t="n">
+        <v>107.13</v>
+      </c>
+      <c r="E187" t="n">
+        <v>99.48999999999999</v>
+      </c>
+      <c r="F187" t="n">
+        <v>63.54</v>
+      </c>
+      <c r="G187" t="n">
+        <v>50.22</v>
+      </c>
+      <c r="H187" t="n">
+        <v>60.49</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2026-01-12 12:52:12</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>NIFTY2611325700CE</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>114</v>
+      </c>
+      <c r="D188" t="n">
+        <v>108.3</v>
+      </c>
+      <c r="E188" t="n">
+        <v>101.89</v>
+      </c>
+      <c r="F188" t="n">
+        <v>62.1</v>
+      </c>
+      <c r="G188" t="n">
+        <v>49.05</v>
+      </c>
+      <c r="H188" t="n">
+        <v>61.26</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2026-01-13 10:09:04</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>NIFTY2612025950CE</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>94.40000000000001</v>
+      </c>
+      <c r="D189" t="n">
+        <v>89.84</v>
+      </c>
+      <c r="E189" t="n">
+        <v>86.73</v>
+      </c>
+      <c r="F189" t="n">
+        <v>59.2</v>
+      </c>
+      <c r="G189" t="n">
+        <v>15.33</v>
+      </c>
+      <c r="H189" t="n">
+        <v>97.11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>